<commit_message>
Added corne keyboard config
</commit_message>
<xml_diff>
--- a/background/Cheatsheet-background.xlsx
+++ b/background/Cheatsheet-background.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portfolio\.config-backup\background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1C6798-9B16-4264-BDE6-3774506092B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06735E2-37F1-4FA4-A924-7C3037461620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABB29E70-2719-4308-A291-2B40FFE59DC1}"/>
   </bookViews>
@@ -283,9 +283,6 @@
     <t>File preview</t>
   </si>
   <si>
-    <t>//</t>
-  </si>
-  <si>
     <t>Buffers</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>Focus Preview Tab</t>
+  </si>
+  <si>
+    <t>\\</t>
   </si>
 </sst>
 </file>
@@ -778,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -810,10 +810,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -844,7 +840,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,7 +1192,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="33"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -1203,26 +1201,26 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="18" t="s">
         <v>56</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="16"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
@@ -1230,47 +1228,47 @@
         <v>31</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="28" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="16"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="23"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="7" t="s">
         <v>27</v>
       </c>
@@ -1280,17 +1278,17 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="23"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="7" t="s">
         <v>29</v>
       </c>
@@ -1298,23 +1296,23 @@
         <v>45</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1325,20 +1323,20 @@
       <c r="H7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1349,20 +1347,20 @@
       <c r="H8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="7" t="s">
         <v>32</v>
       </c>
@@ -1373,20 +1371,20 @@
       <c r="H9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="7" t="s">
         <v>34</v>
       </c>
@@ -1397,20 +1395,20 @@
       <c r="H10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="7" t="s">
         <v>36</v>
       </c>
@@ -1421,38 +1419,38 @@
       <c r="H11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="16"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="22"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="7" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="28"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" s="16"/>
+        <v>90</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="7" t="s">
         <v>46</v>
       </c>
@@ -1460,61 +1458,61 @@
         <v>39</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="16"/>
+      <c r="I13" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="31" t="s">
+      <c r="G15" s="1"/>
+      <c r="H15" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -1527,266 +1525,266 @@
       <c r="H16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="19" t="s">
-        <v>112</v>
+      <c r="B17" s="17" t="s">
+        <v>111</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="19" t="s">
-        <v>137</v>
+      <c r="E17" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="29"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="16"/>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I18" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="J18" s="16"/>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="23"/>
+      <c r="B20" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="26"/>
+      <c r="H20" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="16"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="7" t="s">
+      <c r="I20" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="23"/>
+      <c r="B21" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="7" t="s">
+      <c r="C21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I20" s="18" t="s">
+      <c r="F21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="26"/>
+      <c r="H21" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="J20" s="16"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
-      <c r="B21" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23"/>
+      <c r="B22" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
-      <c r="B22" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" s="16"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="23"/>
+      <c r="B24" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="17" t="s">
+      <c r="C24" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
-      <c r="B24" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="I24" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="23"/>
+      <c r="B25" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="17" t="s">
+      <c r="F25" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="I25" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="23"/>
+      <c r="B26" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F25" s="4" t="s">
+      <c r="C26" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="17" t="s">
+      <c r="F26" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I26" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="23"/>
+      <c r="B27" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="I27" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="J27" s="16"/>
+      <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
@@ -1798,40 +1796,40 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="16"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="22"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="7" t="s">
         <v>48</v>
       </c>
@@ -1844,10 +1842,10 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="16"/>
+      <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="7" t="s">
         <v>49</v>
       </c>
@@ -1859,11 +1857,11 @@
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="16"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="22"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="7" t="s">
         <v>51</v>
       </c>
@@ -1875,8 +1873,8 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="16"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
@@ -1888,7 +1886,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="16"/>
+      <c r="J34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1924,7 +1922,7 @@
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1"/>
@@ -1942,90 +1940,90 @@
     <row r="4" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2038,7 +2036,7 @@
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2046,47 +2044,47 @@
     <row r="15" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>26</v>
@@ -2096,40 +2094,40 @@
     <row r="20" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2169,7 +2167,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2"/>
@@ -2177,7 +2175,7 @@
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2185,30 +2183,30 @@
     <row r="5" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2"/>
     </row>

</xml_diff>